<commit_message>
Import scoring tables and concatenate teams and places
</commit_message>
<xml_diff>
--- a/regattaLinks.xlsx
+++ b/regattaLinks.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>Link</t>
   </si>
@@ -37,6 +37,117 @@
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>harry anderson</t>
+  </si>
+  <si>
+    <t>toni duestch</t>
+  </si>
+  <si>
+    <t>W B</t>
+  </si>
+  <si>
+    <t>penobscot bay</t>
+  </si>
+  <si>
+    <t>Coed B</t>
+  </si>
+  <si>
+    <t>pine trophy</t>
+  </si>
+  <si>
+    <t>harman trophy</t>
+  </si>
+  <si>
+    <t>Coded B</t>
+  </si>
+  <si>
+    <t>mt hope invite</t>
+  </si>
+  <si>
+    <t>Coed C</t>
+  </si>
+  <si>
+    <t>hatch brown</t>
+  </si>
+  <si>
+    <t>regis trophy</t>
+  </si>
+  <si>
+    <t>barnett trophy</t>
+  </si>
+  <si>
+    <t>hoyt trophy</t>
+  </si>
+  <si>
+    <t>hood trophy</t>
+  </si>
+  <si>
+    <t>ms hurst</t>
+  </si>
+  <si>
+    <t>W A</t>
+  </si>
+  <si>
+    <t>norm reid</t>
+  </si>
+  <si>
+    <t>salt pond</t>
+  </si>
+  <si>
+    <t>Womens Showcase 1</t>
+  </si>
+  <si>
+    <t>Womens Showcase 2</t>
+  </si>
+  <si>
+    <t>Danmark</t>
+  </si>
+  <si>
+    <t>moody</t>
+  </si>
+  <si>
+    <t>smith trophy</t>
+  </si>
+  <si>
+    <t>loder trophy</t>
+  </si>
+  <si>
+    <t>coed Showcase1</t>
+  </si>
+  <si>
+    <t>coed showcase 2</t>
+  </si>
+  <si>
+    <t>stu nelson trophy</t>
+  </si>
+  <si>
+    <t>heuitt</t>
+  </si>
+  <si>
+    <t>sister esther</t>
+  </si>
+  <si>
+    <t>great herring pond</t>
+  </si>
+  <si>
+    <t>captain hurst</t>
+  </si>
+  <si>
+    <t>ross trophy</t>
+  </si>
+  <si>
+    <t>shu trophy</t>
+  </si>
+  <si>
+    <t>yale womens</t>
+  </si>
+  <si>
+    <t>oberg trophy</t>
+  </si>
+  <si>
+    <t>fairfield cup</t>
   </si>
 </sst>
 </file>
@@ -367,44 +478,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>